<commit_message>
Removed lingering french values
</commit_message>
<xml_diff>
--- a/data/AI-Survey-Results-tr.xlsx
+++ b/data/AI-Survey-Results-tr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbeltrami/Desktop/Work/Code/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4C88CA-8C5D-2F44-9F9F-ECEB5182DCDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C14103C-19C7-B042-8351-2227142F4B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="1280" windowWidth="14900" windowHeight="21560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4280" yWindow="880" windowWidth="14900" windowHeight="21560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23497" uniqueCount="1166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23497" uniqueCount="1165">
   <si>
     <t>Language</t>
   </si>
@@ -3526,9 +3526,6 @@
   </si>
   <si>
     <t>Maintenant c'est un outil officiel de ma trousse. Particulièrement dans la rédaction de textes.</t>
-  </si>
-  <si>
-    <t>Je ne suis pas certain·e</t>
   </si>
   <si>
     <t>Non, mais j'ai une formation sur…</t>
@@ -3966,8 +3963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IR627"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="HT23" workbookViewId="0">
-      <selection activeCell="HX58" sqref="HX58"/>
+    <sheetView tabSelected="1" topLeftCell="HT1" workbookViewId="0">
+      <selection activeCell="HZ8" sqref="HZ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4768,7 +4765,7 @@
         <v>260</v>
       </c>
       <c r="M2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="N2" t="s">
         <v>262</v>
@@ -4983,7 +4980,7 @@
         <v>260</v>
       </c>
       <c r="M3" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="N3" t="s">
         <v>262</v>
@@ -5073,7 +5070,7 @@
         <v>275</v>
       </c>
       <c r="EA3" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="EB3" t="s">
         <v>274</v>
@@ -5145,7 +5142,7 @@
         <v>3</v>
       </c>
       <c r="IP3" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="IQ3" t="s">
         <v>275</v>
@@ -5225,7 +5222,7 @@
         <v>5</v>
       </c>
       <c r="II4" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="IJ4">
         <v>5</v>
@@ -5246,7 +5243,7 @@
         <v>5</v>
       </c>
       <c r="IQ4" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="5" spans="1:252" x14ac:dyDescent="0.2">
@@ -5547,22 +5544,22 @@
         <v>275</v>
       </c>
       <c r="DY6" t="s">
+        <v>1156</v>
+      </c>
+      <c r="DZ6" t="s">
+        <v>274</v>
+      </c>
+      <c r="EB6" t="s">
+        <v>274</v>
+      </c>
+      <c r="EM6" t="s">
+        <v>274</v>
+      </c>
+      <c r="FS6" t="s">
+        <v>275</v>
+      </c>
+      <c r="GO6" t="s">
         <v>1157</v>
-      </c>
-      <c r="DZ6" t="s">
-        <v>274</v>
-      </c>
-      <c r="EB6" t="s">
-        <v>274</v>
-      </c>
-      <c r="EM6" t="s">
-        <v>274</v>
-      </c>
-      <c r="FS6" t="s">
-        <v>275</v>
-      </c>
-      <c r="GO6" t="s">
-        <v>1158</v>
       </c>
       <c r="GY6" t="s">
         <v>311</v>
@@ -5580,7 +5577,7 @@
         <v>338</v>
       </c>
       <c r="HW6" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="HX6" t="s">
         <v>270</v>
@@ -5732,7 +5729,7 @@
         <v>275</v>
       </c>
       <c r="DY7" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="DZ7" t="s">
         <v>274</v>
@@ -5872,7 +5869,7 @@
         <v>275</v>
       </c>
       <c r="DY8" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="DZ8" t="s">
         <v>274</v>
@@ -5935,7 +5932,7 @@
         <v>391</v>
       </c>
       <c r="HZ8" t="s">
-        <v>1142</v>
+        <v>280</v>
       </c>
       <c r="IB8">
         <v>4</v>
@@ -13180,7 +13177,7 @@
         <v>274</v>
       </c>
       <c r="IA47" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="IB47">
         <v>2</v>
@@ -13225,7 +13222,7 @@
         <v>5</v>
       </c>
       <c r="IP47" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="IQ47" t="s">
         <v>275</v>
@@ -25343,7 +25340,7 @@
         <v>391</v>
       </c>
       <c r="HZ106" t="s">
-        <v>1142</v>
+        <v>280</v>
       </c>
       <c r="IB106">
         <v>1</v>
@@ -25489,7 +25486,7 @@
         <v>274</v>
       </c>
       <c r="GT107" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="GU107" t="s">
         <v>304</v>
@@ -25551,7 +25548,7 @@
         <v>260</v>
       </c>
       <c r="M108" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="N108" t="s">
         <v>262</v>
@@ -25584,13 +25581,13 @@
         <v>275</v>
       </c>
       <c r="DY108" t="s">
+        <v>1144</v>
+      </c>
+      <c r="DZ108" t="s">
+        <v>275</v>
+      </c>
+      <c r="EA108" t="s">
         <v>1145</v>
-      </c>
-      <c r="DZ108" t="s">
-        <v>275</v>
-      </c>
-      <c r="EA108" t="s">
-        <v>1146</v>
       </c>
       <c r="EB108" t="s">
         <v>274</v>
@@ -25647,7 +25644,7 @@
         <v>279</v>
       </c>
       <c r="HZ108" t="s">
-        <v>1142</v>
+        <v>280</v>
       </c>
       <c r="IB108">
         <v>5</v>
@@ -25671,7 +25668,7 @@
         <v>3</v>
       </c>
       <c r="II108" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="IJ108">
         <v>5</v>
@@ -25924,7 +25921,7 @@
         <v>260</v>
       </c>
       <c r="M110" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="N110" t="s">
         <v>287</v>
@@ -26065,7 +26062,7 @@
         <v>274</v>
       </c>
       <c r="IA110" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="IB110">
         <v>1</v>
@@ -83646,7 +83643,7 @@
         <v>274</v>
       </c>
       <c r="IA399" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="IB399">
         <v>5</v>
@@ -91186,7 +91183,7 @@
         <v>260</v>
       </c>
       <c r="M614" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="N614" t="s">
         <v>287</v>
@@ -91342,7 +91339,7 @@
         <v>277</v>
       </c>
       <c r="M620" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="N620" t="s">
         <v>262</v>
@@ -91394,7 +91391,7 @@
         <v>260</v>
       </c>
       <c r="M622" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="N622" t="s">
         <v>263</v>

</xml_diff>

<commit_message>
Removed lingerin french valyes
</commit_message>
<xml_diff>
--- a/data/AI-Survey-Results-tr.xlsx
+++ b/data/AI-Survey-Results-tr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbeltrami/Desktop/Work/Code/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C14103C-19C7-B042-8351-2227142F4B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52432E4D-CA46-D249-A002-77E07A655F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4280" yWindow="880" windowWidth="14900" windowHeight="21560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23497" uniqueCount="1165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23497" uniqueCount="1164">
   <si>
     <t>Language</t>
   </si>
@@ -3538,9 +3538,6 @@
   </si>
   <si>
     <t>Rédaction de textes ou de courriels.</t>
-  </si>
-  <si>
-    <t>J'y réfléchis</t>
   </si>
   <si>
     <t>Pour inspirer des décors</t>
@@ -3963,8 +3960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IR627"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="HT1" workbookViewId="0">
-      <selection activeCell="HZ8" sqref="HZ8"/>
+    <sheetView tabSelected="1" topLeftCell="IC1" workbookViewId="0">
+      <selection activeCell="II4" sqref="II4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4765,7 +4762,7 @@
         <v>260</v>
       </c>
       <c r="M2" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="N2" t="s">
         <v>262</v>
@@ -4980,7 +4977,7 @@
         <v>260</v>
       </c>
       <c r="M3" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="N3" t="s">
         <v>262</v>
@@ -5070,7 +5067,7 @@
         <v>275</v>
       </c>
       <c r="EA3" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="EB3" t="s">
         <v>274</v>
@@ -5142,7 +5139,7 @@
         <v>3</v>
       </c>
       <c r="IP3" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="IQ3" t="s">
         <v>275</v>
@@ -5222,7 +5219,7 @@
         <v>5</v>
       </c>
       <c r="II4" t="s">
-        <v>1146</v>
+        <v>318</v>
       </c>
       <c r="IJ4">
         <v>5</v>
@@ -5243,7 +5240,7 @@
         <v>5</v>
       </c>
       <c r="IQ4" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="5" spans="1:252" x14ac:dyDescent="0.2">
@@ -5544,22 +5541,22 @@
         <v>275</v>
       </c>
       <c r="DY6" t="s">
+        <v>1155</v>
+      </c>
+      <c r="DZ6" t="s">
+        <v>274</v>
+      </c>
+      <c r="EB6" t="s">
+        <v>274</v>
+      </c>
+      <c r="EM6" t="s">
+        <v>274</v>
+      </c>
+      <c r="FS6" t="s">
+        <v>275</v>
+      </c>
+      <c r="GO6" t="s">
         <v>1156</v>
-      </c>
-      <c r="DZ6" t="s">
-        <v>274</v>
-      </c>
-      <c r="EB6" t="s">
-        <v>274</v>
-      </c>
-      <c r="EM6" t="s">
-        <v>274</v>
-      </c>
-      <c r="FS6" t="s">
-        <v>275</v>
-      </c>
-      <c r="GO6" t="s">
-        <v>1157</v>
       </c>
       <c r="GY6" t="s">
         <v>311</v>
@@ -5577,7 +5574,7 @@
         <v>338</v>
       </c>
       <c r="HW6" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="HX6" t="s">
         <v>270</v>
@@ -5729,7 +5726,7 @@
         <v>275</v>
       </c>
       <c r="DY7" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="DZ7" t="s">
         <v>274</v>
@@ -5869,7 +5866,7 @@
         <v>275</v>
       </c>
       <c r="DY8" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="DZ8" t="s">
         <v>274</v>
@@ -13177,7 +13174,7 @@
         <v>274</v>
       </c>
       <c r="IA47" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="IB47">
         <v>2</v>
@@ -13222,7 +13219,7 @@
         <v>5</v>
       </c>
       <c r="IP47" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="IQ47" t="s">
         <v>275</v>
@@ -25668,7 +25665,7 @@
         <v>3</v>
       </c>
       <c r="II108" t="s">
-        <v>1146</v>
+        <v>318</v>
       </c>
       <c r="IJ108">
         <v>5</v>
@@ -25921,7 +25918,7 @@
         <v>260</v>
       </c>
       <c r="M110" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="N110" t="s">
         <v>287</v>
@@ -26062,7 +26059,7 @@
         <v>274</v>
       </c>
       <c r="IA110" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="IB110">
         <v>1</v>
@@ -83643,7 +83640,7 @@
         <v>274</v>
       </c>
       <c r="IA399" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="IB399">
         <v>5</v>
@@ -91183,7 +91180,7 @@
         <v>260</v>
       </c>
       <c r="M614" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="N614" t="s">
         <v>287</v>
@@ -91339,7 +91336,7 @@
         <v>277</v>
       </c>
       <c r="M620" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="N620" t="s">
         <v>262</v>
@@ -91391,7 +91388,7 @@
         <v>260</v>
       </c>
       <c r="M622" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="N622" t="s">
         <v>263</v>

</xml_diff>